<commit_message>
Improve product compatibility logic and address whitelist overrides
Fixes issue with whitelist application and adds a test case for bathtub product searches.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: a7aa588d-1f80-42db-be63-c6c7b4920eb3
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/873c23c0-c18f-4e09-9f8d-38c5cb319996/3688ed1d-aaba-44cd-a054-6cf9d2c9a3f9.jpg
</commit_message>
<xml_diff>
--- a/data/compatibility_whitelist.xlsx
+++ b/data/compatibility_whitelist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bathcraft-my.sharepoint.com/personal/olep00903843_maax_com/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="8_{206B7547-17BE-4FFB-8347-6BD8EE67B904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0423D6FA-778D-4087-BF9E-D0A1D1B2AF6F}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="8_{206B7547-17BE-4FFB-8347-6BD8EE67B904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{20E389D9-6859-426E-99AC-B9E6EA9B894F}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-2730" windowWidth="38640" windowHeight="21120" xr2:uid="{8EDA3920-48F0-4724-A969-C48E638174CB}"/>
+    <workbookView xWindow="46890" yWindow="2775" windowWidth="11895" windowHeight="13350" xr2:uid="{8EDA3920-48F0-4724-A969-C48E638174CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -94,10 +94,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -417,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF02477C-32F7-4DE6-8DE1-53F2FC666413}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -436,6 +432,14 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>105546</v>
+      </c>
+      <c r="B2">
+        <v>139398</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Show users available walls and combination items for base products
Adds logging to troubleshoot why walls and combo items are missing for bases.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: a7aa588d-1f80-42db-be63-c6c7b4920eb3
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/873c23c0-c18f-4e09-9f8d-38c5cb319996/b8e3ad2f-d85f-45dd-a5a7-62ea265d8de6.jpg
</commit_message>
<xml_diff>
--- a/data/compatibility_whitelist.xlsx
+++ b/data/compatibility_whitelist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bathcraft-my.sharepoint.com/personal/olep00903843_maax_com/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="8_{206B7547-17BE-4FFB-8347-6BD8EE67B904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{20E389D9-6859-426E-99AC-B9E6EA9B894F}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="8_{206B7547-17BE-4FFB-8347-6BD8EE67B904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD1ADFE1-4BFB-4F63-B04B-9FCCB03F3E9E}"/>
   <bookViews>
-    <workbookView xWindow="46890" yWindow="2775" windowWidth="11895" windowHeight="13350" xr2:uid="{8EDA3920-48F0-4724-A969-C48E638174CB}"/>
+    <workbookView xWindow="-16980" yWindow="1365" windowWidth="11895" windowHeight="13350" xr2:uid="{8EDA3920-48F0-4724-A969-C48E638174CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -94,6 +94,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -413,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF02477C-32F7-4DE6-8DE1-53F2FC666413}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -432,14 +436,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>105546</v>
-      </c>
-      <c r="B2">
-        <v>139398</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>